<commit_message>
9 Test cases completed BOA
</commit_message>
<xml_diff>
--- a/bankOfAmerica/src/main/resources/BankOfAmericaAutoLoansPageExpectedElements.xlsx
+++ b/bankOfAmerica/src/main/resources/BankOfAmericaAutoLoansPageExpectedElements.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamin\IdeaProjects\AutomationFramework_Team3\bankOfAmerica\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E3110C-4DBD-40F5-B100-995C4F7EA030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECC8DA8-51DA-4FD4-A4EC-2596718E0E64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25860" yWindow="2940" windowWidth="21600" windowHeight="11145" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25860" yWindow="2940" windowWidth="21600" windowHeight="11145" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutoLoansPageTitle" sheetId="1" r:id="rId1"/>
     <sheet name="CarFinancePageTitle" sheetId="2" r:id="rId2"/>
     <sheet name="MenuLinksCount" sheetId="3" r:id="rId3"/>
+    <sheet name="MenuLinks" sheetId="4" r:id="rId4"/>
+    <sheet name="ApplyNow" sheetId="5" r:id="rId5"/>
+    <sheet name="ShopForYourCarNow" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,12 +30,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Auto Loans &amp; Car Financing from Bank of America</t>
   </si>
   <si>
     <t>Learn How Financing a Car Works</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/auto-refinance-loan/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/auto-loan-rates/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/disability-access-loans/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/auto-loan-faq/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/auto-loan-calculator/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/auto-refinance-calculator/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/how-car-loans-work/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/financing-car/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/when-to-refinance-a-car/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/buying-new-or-used-cars/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/auto-loans/lease-buyout/</t>
+  </si>
+  <si>
+    <t>https://secure.bankofamerica.com/applynow/initialize-workflow.go?requesttype=VLSTATUS</t>
+  </si>
+  <si>
+    <t>https://secure.bankofamerica.com/applynow/initialize-workflow.go?requesttype=SNR&amp;flow=AUTO</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/customer-service/contact-us/auto-loans/?topicId=vehicle_oth_loans</t>
+  </si>
+  <si>
+    <t>https://dealer-network.bankofamerica.com/</t>
+  </si>
+  <si>
+    <t>Your Application</t>
+  </si>
+  <si>
+    <t>Shop for a Car and Financing in One Place at Bank of America</t>
   </si>
 </sst>
 </file>
@@ -402,7 +459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B6DE81-1D50-42F0-8BDA-B97A8B038741}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -416,4 +473,143 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE7635D-20BF-4A76-A818-4671CF0BE6F7}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="62.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B20AF93C-533D-4E2D-9A46-59984FD9BFA0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2EA3CE-291F-40AE-A4F9-F5A640E9DBFE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="54.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>